<commit_message>
Corrections in raw data
</commit_message>
<xml_diff>
--- a/Figure 5/5(e,h)/ALD TiN_SEM_processed.xlsx
+++ b/Figure 5/5(e,h)/ALD TiN_SEM_processed.xlsx
@@ -1,19 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E830B392-EC3F-4A62-950A-2DA539B71527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALD TiN SEM overlap" sheetId="1" r:id="rId1"/>
     <sheet name="ALD TiN_conductivity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -391,7 +403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -440,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -450,9 +462,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +742,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3257,11 +3267,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3271,31 +3281,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3306,8 +3316,8 @@
       <c r="B2">
         <v>95526.332699999999</v>
       </c>
-      <c r="C2" s="2">
-        <v>385.20600000000002</v>
+      <c r="C2">
+        <v>382.59999299999998</v>
       </c>
       <c r="D2">
         <v>2.25</v>
@@ -3321,11 +3331,11 @@
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G34" si="1">(C2/B2)*10^6</f>
-        <v>4032.4587902870476</v>
+        <v>4005.1782810667869</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H36" si="2">C2/0.08</f>
-        <v>4815.0749999999998</v>
+        <v>4782.4999124999995</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I36" si="3">F2*SIGN(D2)</f>
@@ -3340,7 +3350,7 @@
         <v>99916</v>
       </c>
       <c r="C3">
-        <v>383.30399999999997</v>
+        <v>380.86066199999999</v>
       </c>
       <c r="D3">
         <v>-8.25</v>
@@ -3354,11 +3364,11 @@
       </c>
       <c r="G3">
         <f t="shared" si="1"/>
-        <v>3836.2624604667917</v>
+        <v>3811.8085391729051</v>
       </c>
       <c r="H3">
         <f t="shared" si="2"/>
-        <v>4791.2999999999993</v>
+        <v>4760.7582750000001</v>
       </c>
       <c r="I3">
         <f t="shared" si="3"/>
@@ -3372,8 +3382,8 @@
       <c r="B4">
         <v>88157.013899999991</v>
       </c>
-      <c r="C4" s="2">
-        <v>363.17700000000002</v>
+      <c r="C4">
+        <v>360.766051</v>
       </c>
       <c r="D4">
         <v>-5.75</v>
@@ -3387,11 +3397,11 @@
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>4119.6608634222366</v>
+        <v>4092.3125119599822</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>4539.7125000000005</v>
+        <v>4509.5756375000001</v>
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
@@ -3406,7 +3416,7 @@
         <v>95228</v>
       </c>
       <c r="C5">
-        <v>372.45499999999998</v>
+        <v>370.18898200000001</v>
       </c>
       <c r="D5">
         <v>7.75</v>
@@ -3420,11 +3430,11 @@
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>3911.1920863611545</v>
+        <v>3887.3963750157518</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>4655.6875</v>
+        <v>4627.3622750000004</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
@@ -3439,7 +3449,7 @@
         <v>97396</v>
       </c>
       <c r="C6">
-        <v>377.65</v>
+        <v>375.33335499999998</v>
       </c>
       <c r="D6">
         <v>9.75</v>
@@ -3453,11 +3463,11 @@
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>3877.4693005872932</v>
+        <v>3853.6834674935312</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>4720.625</v>
+        <v>4691.6669375000001</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
@@ -3472,7 +3482,7 @@
         <v>96310</v>
       </c>
       <c r="C7">
-        <v>397.02029496286298</v>
+        <v>393.972579</v>
       </c>
       <c r="D7">
         <v>13.75</v>
@@ -3486,11 +3496,11 @@
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>4122.316425738376</v>
+        <v>4090.6715709687469</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>4962.7536870357872</v>
+        <v>4924.6572374999996</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
@@ -3504,8 +3514,8 @@
       <c r="B8">
         <v>82796.6976</v>
       </c>
-      <c r="C8" s="2">
-        <v>324.53199999999998</v>
+      <c r="C8">
+        <v>322.33842600000003</v>
       </c>
       <c r="D8">
         <v>-13.75</v>
@@ -3519,11 +3529,11 @@
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>3919.624929581732</v>
+        <v>3893.1314333000651</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>4056.6499999999996</v>
+        <v>4029.2303250000004</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
@@ -3537,8 +3547,8 @@
       <c r="B9">
         <v>91504</v>
       </c>
-      <c r="C9" s="2">
-        <v>374.20800000000003</v>
+      <c r="C9">
+        <v>371.64198699999997</v>
       </c>
       <c r="D9">
         <v>-14.25</v>
@@ -3552,11 +3562,11 @@
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>4089.5261409337295</v>
+        <v>4061.4835089176427</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>4677.6000000000004</v>
+        <v>4645.5248374999992</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
@@ -3570,8 +3580,8 @@
       <c r="B10">
         <v>92813</v>
       </c>
-      <c r="C10" s="2">
-        <v>351.77699999999999</v>
+      <c r="C10">
+        <v>349.65438</v>
       </c>
       <c r="D10">
         <v>-22.25</v>
@@ -3585,11 +3595,11 @@
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>3790.1694805684547</v>
+        <v>3767.2996239750901</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>4397.2124999999996</v>
+        <v>4370.6797500000002</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
@@ -3603,8 +3613,8 @@
       <c r="B11">
         <v>98045</v>
       </c>
-      <c r="C11" s="2">
-        <v>379.43299999999999</v>
+      <c r="C11">
+        <v>376.87962499999998</v>
       </c>
       <c r="D11">
         <v>-16.25</v>
@@ -3618,11 +3628,11 @@
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>3869.9882706920289</v>
+        <v>3843.9453822224486</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>4742.9124999999995</v>
+        <v>4710.9953124999993</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
@@ -3637,7 +3647,7 @@
         <v>87605</v>
       </c>
       <c r="C12">
-        <v>320.62299999999999</v>
+        <v>318.32039400000002</v>
       </c>
       <c r="D12">
         <v>15.75</v>
@@ -3651,11 +3661,11 @@
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>3659.8710119285429</v>
+        <v>3633.5870555333604</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>4007.7874999999999</v>
+        <v>3979.0049250000002</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
@@ -3669,8 +3679,8 @@
       <c r="B13">
         <v>86345.439299999998</v>
       </c>
-      <c r="C13" s="2">
-        <v>350.19799999999998</v>
+      <c r="C13">
+        <v>347.73478</v>
       </c>
       <c r="D13">
         <v>18.25</v>
@@ -3684,11 +3694,11 @@
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>4055.7787746410827</v>
+        <v>4027.2512690777407</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>4377.4749999999995</v>
+        <v>4346.6847500000003</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
@@ -3702,8 +3712,8 @@
       <c r="B14">
         <v>87958</v>
       </c>
-      <c r="C14" s="2">
-        <v>355.66</v>
+      <c r="C14">
+        <v>353.41118399999999</v>
       </c>
       <c r="D14">
         <v>29.75</v>
@@ -3717,11 +3727,11 @@
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>4043.5207712772012</v>
+        <v>4017.953841606221</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>4445.75</v>
+        <v>4417.6397999999999</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
@@ -3735,8 +3745,8 @@
       <c r="B15">
         <v>76224.035099999892</v>
       </c>
-      <c r="C15" s="2">
-        <v>303.42500000000001</v>
+      <c r="C15">
+        <v>301.34893299999999</v>
       </c>
       <c r="D15">
         <v>-21.75</v>
@@ -3750,11 +3760,11 @@
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>3980.6997832367506</v>
+        <v>3953.4634004176514</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>3792.8125</v>
+        <v>3766.8616625</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
@@ -3768,8 +3778,8 @@
       <c r="B16">
         <v>81231</v>
       </c>
-      <c r="C16" s="2">
-        <v>300.31299999999999</v>
+      <c r="C16">
+        <v>298.35282699999999</v>
       </c>
       <c r="D16">
         <v>23.75</v>
@@ -3783,11 +3793,11 @@
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>3697.0245349681772</v>
+        <v>3672.8936859080891</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>3753.9124999999999</v>
+        <v>3729.4103375</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
@@ -3801,8 +3811,8 @@
       <c r="B17">
         <v>88952</v>
       </c>
-      <c r="C17" s="2">
-        <v>329.92099999999999</v>
+      <c r="C17">
+        <v>327.83011499999998</v>
       </c>
       <c r="D17">
         <v>-24.25</v>
@@ -3816,11 +3826,11 @@
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>3708.9778757082472</v>
+        <v>3685.4721085529272</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>4124.0124999999998</v>
+        <v>4097.8764375000001</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
@@ -3834,8 +3844,8 @@
       <c r="B18">
         <v>80773.805699999997</v>
       </c>
-      <c r="C18" s="2">
-        <v>325.59399999999999</v>
+      <c r="C18">
+        <v>323.36190099999999</v>
       </c>
       <c r="D18">
         <v>30.25</v>
@@ -3849,11 +3859,11 @@
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>4030.9354892758261</v>
+        <v>4003.3015430892342</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>4069.9249999999997</v>
+        <v>4042.0237625</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
@@ -3867,8 +3877,8 @@
       <c r="B19">
         <v>74579</v>
       </c>
-      <c r="C19" s="2">
-        <v>283.46300000000002</v>
+      <c r="C19">
+        <v>281.89321899999999</v>
       </c>
       <c r="D19">
         <v>-30.25</v>
@@ -3882,11 +3892,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>3800.8420600973468</v>
+        <v>3779.7934941471458</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>3543.2875000000004</v>
+        <v>3523.6652374999999</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
@@ -3900,8 +3910,8 @@
       <c r="B20">
         <v>85516</v>
       </c>
-      <c r="C20" s="2">
-        <v>276.83699999999999</v>
+      <c r="C20">
+        <v>275.018033</v>
       </c>
       <c r="D20">
         <v>27.75</v>
@@ -3915,46 +3925,46 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>3237.2538472332658</v>
+        <v>3215.9833598390946</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>3460.4624999999996</v>
+        <v>3437.7254124999999</v>
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
         <v>43.693534990888523</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21">
         <v>86745</v>
       </c>
-      <c r="C21" s="9">
-        <v>285.53059999999999</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21">
+        <v>283.72517699999997</v>
+      </c>
+      <c r="D21">
         <v>21.75</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21">
         <v>34.25</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21">
         <f t="shared" si="0"/>
         <v>40.572466033013079</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21">
         <f t="shared" si="1"/>
-        <v>3291.6087382558071</v>
-      </c>
-      <c r="H21" s="7">
+        <v>3270.7957461525157</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="2"/>
-        <v>3569.1324999999997</v>
-      </c>
-      <c r="I21" s="7">
+        <v>3546.5647124999996</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="3"/>
         <v>40.572466033013079</v>
       </c>
@@ -3966,8 +3976,8 @@
       <c r="B22">
         <v>93597.6902999999</v>
       </c>
-      <c r="C22" s="2">
-        <v>364.01389999999998</v>
+      <c r="C22">
+        <v>361.77751899999998</v>
       </c>
       <c r="D22">
         <v>9.75</v>
@@ -3981,11 +3991,11 @@
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>3889.1333625141856</v>
+        <v>3865.2398135085218</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>4550.1737499999999</v>
+        <v>4522.2189874999995</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
@@ -3999,8 +4009,8 @@
       <c r="B23">
         <v>89704.689899999998</v>
       </c>
-      <c r="C23" s="2">
-        <v>339.512</v>
+      <c r="C23">
+        <v>328.60957000000002</v>
       </c>
       <c r="D23">
         <v>-32.25</v>
@@ -4014,11 +4024,11 @@
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>3784.7742451200425</v>
+        <v>3663.2373442940802</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>4243.8999999999996</v>
+        <v>4107.6196250000003</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
@@ -4032,8 +4042,8 @@
       <c r="B24">
         <v>90051.924899999998</v>
       </c>
-      <c r="C24" s="2">
-        <v>334.81900000000002</v>
+      <c r="C24">
+        <v>332.90978000000001</v>
       </c>
       <c r="D24">
         <v>-26.25</v>
@@ -4047,11 +4057,11 @@
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>3718.0659977208329</v>
+        <v>3696.8646741275825</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>4185.2375000000002</v>
+        <v>4161.3722500000003</v>
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
@@ -4065,8 +4075,8 @@
       <c r="B25">
         <v>83763.002999999997</v>
       </c>
-      <c r="C25" s="2">
-        <v>281.54899999999998</v>
+      <c r="C25">
+        <v>279.81870800000002</v>
       </c>
       <c r="D25">
         <v>-34.25</v>
@@ -4080,11 +4090,11 @@
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>3361.2572366824047</v>
+        <v>3340.6002408963304</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>3519.3624999999997</v>
+        <v>3497.7338500000001</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
@@ -4098,8 +4108,8 @@
       <c r="B26">
         <v>89941.801800000001</v>
       </c>
-      <c r="C26" s="2">
-        <v>337.71800000000002</v>
+      <c r="C26">
+        <v>335.69217200000003</v>
       </c>
       <c r="D26">
         <v>-24.25</v>
@@ -4113,11 +4123,11 @@
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>3754.8502836419721</v>
+        <v>3732.3265187244674</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>4221.4750000000004</v>
+        <v>4196.1521499999999</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
@@ -4131,8 +4141,8 @@
       <c r="B27">
         <v>98852.843999999997</v>
       </c>
-      <c r="C27" s="2">
-        <v>381.20699999999999</v>
+      <c r="C27">
+        <v>378.53232400000002</v>
       </c>
       <c r="D27">
         <v>3.75</v>
@@ -4146,11 +4156,11 @@
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>3856.3078670756304</v>
+        <v>3829.250719382439</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>4765.0874999999996</v>
+        <v>4731.6540500000001</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
@@ -4158,14 +4168,14 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
+      <c r="A28" t="s">
         <v>83</v>
       </c>
       <c r="B28">
         <v>90499.361999999994</v>
       </c>
-      <c r="C28" s="2">
-        <v>350.94099999999997</v>
+      <c r="C28">
+        <v>348.51854100000003</v>
       </c>
       <c r="D28">
         <v>23.75</v>
@@ -4179,11 +4189,11 @@
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>3877.8284425916727</v>
+        <v>3851.0607511244116</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>4386.7624999999998</v>
+        <v>4356.4817625000005</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
@@ -4191,14 +4201,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
+      <c r="A29" t="s">
         <v>77</v>
       </c>
       <c r="B29">
         <v>87557.785499999998</v>
       </c>
-      <c r="C29" s="2">
-        <v>344.71699999999998</v>
+      <c r="C29">
+        <v>342.366196</v>
       </c>
       <c r="D29">
         <v>25.75</v>
@@ -4212,11 +4222,11 @@
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>3937.0228247721038</v>
+        <v>3910.1742243126969</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>4308.9624999999996</v>
+        <v>4279.5774499999998</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
@@ -4224,14 +4234,14 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
+      <c r="A30" t="s">
         <v>84</v>
       </c>
       <c r="B30">
         <v>86835.536699999997</v>
       </c>
-      <c r="C30" s="2">
-        <v>331.05399999999997</v>
+      <c r="C30">
+        <v>329.00780500000002</v>
       </c>
       <c r="D30">
         <v>-20.25</v>
@@ -4245,11 +4255,11 @@
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>3812.4253339243769</v>
+        <v>3788.8613061338979</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>4138.1749999999993</v>
+        <v>4112.5975625000001</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
@@ -4257,14 +4267,14 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
+      <c r="A31" t="s">
         <v>54</v>
       </c>
       <c r="B31">
         <v>98587.953299999994</v>
       </c>
-      <c r="C31" s="2">
-        <v>365.39299999999997</v>
+      <c r="C31">
+        <v>362.90587499999998</v>
       </c>
       <c r="D31">
         <v>-6.25</v>
@@ -4278,11 +4288,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>3706.2641810619675</v>
+        <v>3681.0367073519519</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>4567.4124999999995</v>
+        <v>4536.3234374999993</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
@@ -4290,14 +4300,14 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>86</v>
       </c>
       <c r="B32">
         <v>81758.960999999996</v>
       </c>
-      <c r="C32" s="2">
-        <v>313.71699999999998</v>
+      <c r="C32">
+        <v>311.83471500000002</v>
       </c>
       <c r="D32">
         <v>-28.25</v>
@@ -4311,11 +4321,11 @@
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>3837.0962175020791</v>
+        <v>3814.0738481253452</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>3921.4624999999996</v>
+        <v>3897.9339375</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
@@ -4323,14 +4333,14 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>87</v>
       </c>
       <c r="B33">
         <v>73206.066899999903</v>
       </c>
-      <c r="C33" s="2">
-        <v>284.66500000000002</v>
+      <c r="C33">
+        <v>283.00771300000002</v>
       </c>
       <c r="D33">
         <v>31.75</v>
@@ -4344,11 +4354,11 @@
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>3888.5438332434223</v>
+        <v>3865.9051767743636</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>3558.3125</v>
+        <v>3537.5964125</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
@@ -4356,14 +4366,14 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+      <c r="A34" t="s">
         <v>88</v>
       </c>
       <c r="B34">
         <v>90617.421900000001</v>
       </c>
-      <c r="C34" s="2">
-        <v>347.62400000000002</v>
+      <c r="C34">
+        <v>345.32294899999999</v>
       </c>
       <c r="D34">
         <v>-12.25</v>
@@ -4377,11 +4387,11 @@
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>3836.1718167574572</v>
+        <v>3810.7787857954936</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>4345.3</v>
+        <v>4316.5368625000001</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
@@ -4389,14 +4399,14 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
+      <c r="A35" t="s">
         <v>89</v>
       </c>
       <c r="B35">
         <v>88895.136299999896</v>
       </c>
-      <c r="C35" s="2">
-        <v>355.988</v>
+      <c r="C35">
+        <v>353.65588200000002</v>
       </c>
       <c r="D35">
         <v>27.75</v>
@@ -4410,11 +4420,11 @@
       </c>
       <c r="G35">
         <f>(C35/B35)*10^6</f>
-        <v>4004.5835443530382</v>
+        <v>3978.3490607010908</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>4449.8499999999995</v>
+        <v>4420.6985249999998</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
@@ -4422,14 +4432,14 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="7" t="s">
+      <c r="A36" t="s">
         <v>120</v>
       </c>
       <c r="B36">
         <v>88535.003999999899</v>
       </c>
-      <c r="C36" s="2">
-        <v>350.09269999999998</v>
+      <c r="C36">
+        <v>347.76735200000002</v>
       </c>
       <c r="D36">
         <v>21.75</v>
@@ -4443,11 +4453,11 @@
       </c>
       <c r="G36">
         <f>(C36/B36)*10^6</f>
-        <v>3954.2856969882823</v>
+        <v>3928.020966712786</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>4376.1587499999996</v>
+        <v>4347.0919000000004</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
@@ -4455,7 +4465,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I45">
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>